<commit_message>
New NEON products supported: Elevation of surface water, elevation of groundwater.
</commit_message>
<xml_diff>
--- a/NEON/NEONHarvester/settings/neon_variables_lookup.xlsx
+++ b/NEON/NEONHarvester/settings/neon_variables_lookup.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="139">
   <si>
     <t xml:space="preserve">ProductCode</t>
   </si>
@@ -181,30 +181,30 @@
     <t xml:space="preserve">kilopascal</t>
   </si>
   <si>
-    <t xml:space="preserve">corPresMean</t>
+    <t xml:space="preserve">corPres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.00004.001_corPres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.00005.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR biological temperature </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRBT_30_minute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bioTempMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.neonscience.org/api/v0/documents/NEON.DOC.000652vA</t>
   </si>
   <si>
     <t xml:space="preserve">no</t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.00004.001_corPresMean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DP1.00005.001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IR biological temperature </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IRBT_30_minute</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bioTempMean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://data.neonscience.org/api/v0/documents/NEON.DOC.000652vA</t>
-  </si>
-  <si>
     <t xml:space="preserve">?</t>
   </si>
   <si>
@@ -359,6 +359,102 @@
   </si>
   <si>
     <t xml:space="preserve">dimensionless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.20046.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air temperature above water on-buoy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rhbuoy_30min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tempRHMean</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">http://data.neonscience.org/data-product-view?dpCode=DP1.20046</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">.001</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.20271.001_tempRHMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.20004.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barometric pressure above water on-buoy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.20004.001_staPresMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.20004.001_corPres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.20100.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elevation of groundwater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EOG_30_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">groundwaterElevMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.neonscience.org/data-product-view?dpCode=DP1.20100.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.20100.001_groundwaterElevMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groundwater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.20016.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elevation of surface water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EOS_30_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">surfacewaterElevMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.neonscience.org/data-product-view?dpCode=DP1.20016.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.20016.001_surfacewaterElevMean</t>
   </si>
 </sst>
 </file>
@@ -368,7 +464,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -391,6 +487,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="238"/>
     </font>
   </fonts>
@@ -436,7 +539,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -447,6 +550,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -466,10 +573,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -483,7 +590,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17"/>
@@ -774,10 +881,10 @@
         <v>49</v>
       </c>
       <c r="G7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>55</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>46</v>
@@ -800,25 +907,25 @@
     </row>
     <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="0" t="s">
+      <c r="E8" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>61</v>
@@ -950,7 +1057,7 @@
         <v>76</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>61</v>
@@ -967,7 +1074,7 @@
         <v>79</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>61</v>
@@ -984,7 +1091,7 @@
         <v>79</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>61</v>
@@ -1007,7 +1114,7 @@
         <v>85</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>61</v>
@@ -1075,7 +1182,7 @@
       </c>
       <c r="D16" s="1"/>
       <c r="G16" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="I16" s="0" t="s">
         <v>61</v>
@@ -1169,7 +1276,232 @@
         <v>137</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N20" s="1" t="n">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N21" s="1" t="n">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F19" r:id="rId1" display="http://data.neonscience.org/data-product-view?dpCode=DP1.20046"/>
+    <hyperlink ref="F22" r:id="rId2" display="http://data.neonscience.org/data-product-view?dpCode=DP1.20100.001"/>
+    <hyperlink ref="F23" r:id="rId3" display="http://data.neonscience.org/data-product-view?dpCode=DP1.20016.001"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
New NEON products and CUAHSI variables added to lookup table.
</commit_message>
<xml_diff>
--- a/NEON/NEONHarvester/settings/neon_variables_lookup.xlsx
+++ b/NEON/NEONHarvester/settings/neon_variables_lookup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="neon_variables" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="163">
   <si>
     <t xml:space="preserve">ProductCode</t>
   </si>
@@ -202,87 +202,66 @@
     <t xml:space="preserve">http://data.neonscience.org/api/v0/documents/NEON.DOC.000652vA</t>
   </si>
   <si>
+    <t xml:space="preserve">DP1.00005.001_bioTempMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.00006.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precipitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIPRE_30min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">priPrecipBulk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.neonscience.org/api/v0/documents/NEON.DOC.000898_DRAFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.00006.001_priPrecipBulk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">millimeter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SECPRE_30min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secPrecipBulk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.neonscience.org/api/v0/documents/NEON.DOC.000816vA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.00006.001_secPrecipBulk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paused</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THRPRE_30min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFPrecipBulk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.neonscience.org/api/v0/documents/NEON.DOC.001300vB</t>
+  </si>
+  <si>
     <t xml:space="preserve">no</t>
   </si>
   <si>
     <t xml:space="preserve">?</t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.00006.001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precipitation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIPRE_30min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">priPrecipBulk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://data.neonscience.org/api/v0/documents/NEON.DOC.000898_DRAFT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DP1.00006.001_priPrecipBulk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">millimeter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SECPRE_30min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">secPrecipBulk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://data.neonscience.org/api/v0/documents/NEON.DOC.000816vA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DP1.00006.001_secPrecipBulk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paused</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THRPRE_30min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TFPrecipBulk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://data.neonscience.org/api/v0/documents/NEON.DOC.001300vB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DP1.00007.001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3D wind speed, direction and sonic temperature </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FUTURE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DP1.00010.001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3D wind attitude and motion reference </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DP1.00013.001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wet deposition chemical analysis </t>
-  </si>
-  <si>
-    <t xml:space="preserve">wdp_chemLab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">precipCalcium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">milligrams per liter</t>
-  </si>
-  <si>
     <t xml:space="preserve">DP1.00014.001</t>
   </si>
   <si>
@@ -307,12 +286,6 @@
     <t xml:space="preserve">watts per square meter </t>
   </si>
   <si>
-    <t xml:space="preserve">DP1.00017.001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dust and particulate size distribution </t>
-  </si>
-  <si>
     <t xml:space="preserve">DP1.00041.001</t>
   </si>
   <si>
@@ -373,25 +346,7 @@
     <t xml:space="preserve">tempRHMean</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">http://data.neonscience.org/data-product-view?dpCode=DP1.20046</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">.001</t>
-    </r>
+    <t xml:space="preserve">http://data.neonscience.org/data-product-view?dpCode=DP1.20046.001</t>
   </si>
   <si>
     <t xml:space="preserve">DP1.20271.001_tempRHMean</t>
@@ -455,6 +410,105 @@
   </si>
   <si>
     <t xml:space="preserve">DP1.20016.001_surfacewaterElevMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.00024.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photosynthetically active radiation (PAR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARPAR_30min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.neonscience.org/data-product-view?dpCode=DP1.00024.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.00024.001_PARMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radiation, incoming PAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.00066.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photosynthetically active radiation (quantum line)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARQL_30min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linePARMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.neonscience.org/data-product-view?dpCode=DP1.00166.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.00066.001_linePARMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.20242.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARWS_30min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.neonscience.org/data-product-view?dpCode=DP1.20042.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.20042.001_PARMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.20261.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uPAR_30min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uPARMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.neonscience.org/data-product-view?dpCode=DP1.20261.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.20261.001_uPARMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.00098.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relative humidity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RH_30min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RHMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.neonscience.org/data-product-view?dpCode=DP1.00098.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.00098.001_RHMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.20271.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relative humidity above water on-buoy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.neonscience.org/data-product-view?dpCode=DP1.20271.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DP1.20271.001_RHMean</t>
   </si>
 </sst>
 </file>
@@ -464,7 +518,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -475,26 +529,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -539,7 +583,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -550,10 +594,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -573,35 +613,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N65536"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="61.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="60.8826530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -641,7 +681,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -685,11 +725,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -905,7 +945,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>55</v>
       </c>
@@ -925,19 +965,19 @@
         <v>59</v>
       </c>
       <c r="G8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="I8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="K8" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>25</v>
@@ -951,43 +991,43 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>63</v>
       </c>
       <c r="J9" s="0" t="s">
         <v>23</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L9" s="0" t="s">
         <v>25</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N9" s="0" t="n">
         <v>54</v>
@@ -995,43 +1035,43 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>20</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J10" s="0" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>25</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N10" s="0" t="n">
         <v>54</v>
@@ -1039,414 +1079,509 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>79</v>
+        <v>16</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>84</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>85</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>81</v>
+        <v>88</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>89</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>79</v>
+        <v>16</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>92</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>93</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>83</v>
+        <v>37</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>96</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>85</v>
+        <v>97</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>99</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>61</v>
+        <v>20</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="N14" s="0" t="n">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>103</v>
+      </c>
+      <c r="N14" s="2" t="n">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>88</v>
+        <v>104</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>105</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>89</v>
+      <c r="D15" s="0" t="s">
+        <v>106</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>20</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="J15" s="0" t="s">
         <v>23</v>
       </c>
       <c r="K15" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L15" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="N15" s="0" t="n">
+      <c r="L16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N16" s="1" t="n">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N17" s="1" t="n">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="N18" s="0" t="n">
         <v>33</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="G16" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="M17" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="N17" s="0" t="n">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="L18" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="M18" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="N18" s="2" t="n">
-        <v>137</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>128</v>
       </c>
       <c r="G19" s="0" t="s">
         <v>20</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>37</v>
+        <v>121</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="L19" s="0" t="s">
         <v>25</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>38</v>
+        <v>123</v>
       </c>
       <c r="N19" s="0" t="n">
-        <v>96</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>47</v>
+        <v>132</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>48</v>
+        <v>133</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>49</v>
+        <v>134</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N20" s="1" t="n">
-        <v>170</v>
+      <c r="H20" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>47</v>
+        <v>139</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>53</v>
+        <v>140</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>49</v>
+        <v>141</v>
       </c>
       <c r="G21" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N21" s="1" t="n">
-        <v>170</v>
+      <c r="H21" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>128</v>
+        <v>133</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>145</v>
       </c>
       <c r="G22" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>130</v>
+      <c r="H22" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>136</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="L22" s="0" t="s">
         <v>25</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>132</v>
+        <v>87</v>
       </c>
       <c r="N22" s="0" t="n">
         <v>33</v>
@@ -1454,60 +1589,147 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="E23" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I23" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>130</v>
-      </c>
       <c r="J23" s="0" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="L23" s="0" t="s">
         <v>25</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>132</v>
+        <v>87</v>
       </c>
       <c r="N23" s="0" t="n">
         <v>33</v>
       </c>
     </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L24" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M24" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L25" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F19" r:id="rId1" display="http://data.neonscience.org/data-product-view?dpCode=DP1.20046"/>
-    <hyperlink ref="F22" r:id="rId2" display="http://data.neonscience.org/data-product-view?dpCode=DP1.20100.001"/>
-    <hyperlink ref="F23" r:id="rId3" display="http://data.neonscience.org/data-product-view?dpCode=DP1.20016.001"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Stránka &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
corrected variable code and CV in lookup table. Fixed issue with missing secondary precipitation data.
</commit_message>
<xml_diff>
--- a/NEON/NEONHarvester/settings/neon_variables_lookup.xlsx
+++ b/NEON/NEONHarvester/settings/neon_variables_lookup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="neon_variables" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="162">
   <si>
     <t xml:space="preserve">ProductCode</t>
   </si>
@@ -205,9 +205,6 @@
     <t xml:space="preserve">DP1.00005.001_bioTempMean</t>
   </si>
   <si>
-    <t xml:space="preserve">Biota</t>
-  </si>
-  <si>
     <t xml:space="preserve">Other</t>
   </si>
   <si>
@@ -277,7 +274,7 @@
     <t xml:space="preserve">http://data.neonscience.org/api/v0/documents/NEON.DOC.000815vB</t>
   </si>
   <si>
-    <t xml:space="preserve">gloRadMean_SRDDP_30min_00014_001</t>
+    <t xml:space="preserve">DP1.00014.001_gloRadMean</t>
   </si>
   <si>
     <t xml:space="preserve">Global radiation</t>
@@ -529,16 +526,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -613,28 +613,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N65536"/>
+  <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="60.8826530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.3928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="60.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,10 +974,10 @@
         <v>37</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>25</v>
@@ -991,43 +991,43 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="C9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="0" t="s">
+      <c r="E9" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="F9" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="G9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>68</v>
-      </c>
       <c r="I9" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J9" s="0" t="s">
         <v>23</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L9" s="0" t="s">
         <v>25</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N9" s="0" t="n">
         <v>54</v>
@@ -1035,43 +1035,43 @@
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>64</v>
-      </c>
       <c r="C10" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="F10" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="G10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>73</v>
-      </c>
       <c r="I10" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J10" s="0" t="s">
         <v>23</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>25</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N10" s="0" t="n">
         <v>54</v>
@@ -1079,57 +1079,57 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>64</v>
-      </c>
       <c r="C11" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="E11" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="F11" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="G11" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="H11" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="F12" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="G12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="G12" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="0" t="s">
+      <c r="I12" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>86</v>
       </c>
       <c r="J12" s="0" t="s">
         <v>23</v>
@@ -1141,7 +1141,7 @@
         <v>25</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N12" s="0" t="n">
         <v>33</v>
@@ -1149,28 +1149,28 @@
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="C13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="0" t="s">
+      <c r="E13" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="F13" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="G13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>93</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>37</v>
@@ -1179,7 +1179,7 @@
         <v>23</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L13" s="0" t="s">
         <v>25</v>
@@ -1193,43 +1193,43 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="C14" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="0" t="s">
+      <c r="E14" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="G14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="G14" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="0" t="s">
+      <c r="I14" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="J14" s="0" t="s">
+      <c r="K14" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="K14" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="M14" s="0" t="s">
-        <v>103</v>
       </c>
       <c r="N14" s="2" t="n">
         <v>137</v>
@@ -1237,28 +1237,28 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="C15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="0" t="s">
+      <c r="E15" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="F15" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="G15" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>109</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>37</v>
@@ -1267,7 +1267,7 @@
         <v>23</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L15" s="0" t="s">
         <v>25</v>
@@ -1281,10 +1281,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>112</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>16</v>
@@ -1302,7 +1302,7 @@
         <v>20</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>51</v>
@@ -1325,10 +1325,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>112</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>16</v>
@@ -1346,7 +1346,7 @@
         <v>20</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>46</v>
@@ -1369,43 +1369,43 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="C18" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="0" t="s">
+      <c r="E18" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="F18" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="G18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="G18" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="0" t="s">
+      <c r="I18" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="J18" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="K18" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="J18" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="K18" s="0" t="s">
+      <c r="L18" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M18" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="L18" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="M18" s="0" t="s">
-        <v>123</v>
       </c>
       <c r="N18" s="0" t="n">
         <v>33</v>
@@ -1413,43 +1413,43 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="C19" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="0" t="s">
+      <c r="E19" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="F19" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="G19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="G19" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>129</v>
-      </c>
       <c r="I19" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L19" s="0" t="s">
         <v>25</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N19" s="0" t="n">
         <v>33</v>
@@ -1457,43 +1457,43 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="C20" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="0" t="s">
+      <c r="E20" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="F20" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="G20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="G20" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="I20" s="0" t="s">
-        <v>136</v>
-      </c>
       <c r="J20" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="K20" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="L20" s="0" t="s">
         <v>25</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N20" s="0" t="n">
         <v>33</v>
@@ -1501,43 +1501,43 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="C21" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="0" t="s">
+      <c r="E21" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="F21" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="G21" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G21" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="I21" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>94</v>
+        <v>23</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L21" s="0" t="s">
         <v>25</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N21" s="0" t="n">
         <v>33</v>
@@ -1545,43 +1545,43 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="0" t="s">
+      <c r="E22" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="E22" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="F22" s="0" t="s">
+      <c r="G22" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="G22" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="I22" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L22" s="0" t="s">
         <v>25</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N22" s="0" t="n">
         <v>33</v>
@@ -1589,43 +1589,43 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="B23" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="0" t="s">
+      <c r="E23" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="F23" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="G23" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G23" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="I23" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L23" s="0" t="s">
         <v>25</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N23" s="0" t="n">
         <v>33</v>
@@ -1633,31 +1633,31 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B24" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="C24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="0" t="s">
+      <c r="E24" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="F24" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="G24" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="G24" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>157</v>
-      </c>
       <c r="I24" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J24" s="0" t="s">
         <v>23</v>
@@ -1669,7 +1669,7 @@
         <v>25</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N24" s="0" t="n">
         <v>1</v>
@@ -1677,31 +1677,31 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="C25" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="F25" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="F25" s="0" t="s">
+      <c r="G25" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="G25" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>162</v>
-      </c>
       <c r="I25" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J25" s="0" t="s">
         <v>23</v>
@@ -1713,7 +1713,7 @@
         <v>25</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N25" s="0" t="n">
         <v>1</v>
@@ -1726,10 +1726,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Stránka &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new NEONTester project to test the web services.
</commit_message>
<xml_diff>
--- a/NEON/NEONHarvester/settings/neon_variables_lookup.xlsx
+++ b/NEON/NEONHarvester/settings/neon_variables_lookup.xlsx
@@ -223,6 +223,9 @@
     <t xml:space="preserve">http://data.neonscience.org/api/v0/documents/NEON.DOC.000898_DRAFT</t>
   </si>
   <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
     <t xml:space="preserve">DP1.00006.001_priPrecipBulk</t>
   </si>
   <si>
@@ -251,9 +254,6 @@
   </si>
   <si>
     <t xml:space="preserve">http://data.neonscience.org/api/v0/documents/NEON.DOC.001300vB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
   </si>
   <si>
     <t xml:space="preserve">?</t>
@@ -615,8 +615,8 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -628,7 +628,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="60.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.53"/>
@@ -1009,10 +1009,10 @@
         <v>66</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>63</v>
@@ -1027,7 +1027,7 @@
         <v>25</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N9" s="0" t="n">
         <v>54</v>
@@ -1044,19 +1044,19 @@
         <v>16</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>63</v>
@@ -1071,7 +1071,7 @@
         <v>25</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N10" s="0" t="n">
         <v>54</v>
@@ -1085,19 +1085,19 @@
         <v>63</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>78</v>
@@ -1387,7 +1387,7 @@
         <v>118</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>119</v>
@@ -1431,7 +1431,7 @@
         <v>127</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="H19" s="0" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
NEON harvester - method descriptions are taken from lookup .xlsx file.
</commit_message>
<xml_diff>
--- a/NEON/NEONHarvester/settings/neon_variables_lookup.xlsx
+++ b/NEON/NEONHarvester/settings/neon_variables_lookup.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="181">
   <si>
     <t xml:space="preserve">ProductCode</t>
   </si>
@@ -64,6 +64,9 @@
     <t xml:space="preserve">UnitsID</t>
   </si>
   <si>
+    <t xml:space="preserve">MethodDescription</t>
+  </si>
+  <si>
     <t xml:space="preserve">DP1.00001.001</t>
   </si>
   <si>
@@ -103,6 +106,9 @@
     <t xml:space="preserve">meters per second</t>
   </si>
   <si>
+    <t xml:space="preserve">Observations are made by 2-D sonic anemometer sensors located on the aquatic meteorological station and at multiple heights on the tower infrastructure.</t>
+  </si>
+  <si>
     <t xml:space="preserve">windDirMean</t>
   </si>
   <si>
@@ -139,6 +145,9 @@
     <t xml:space="preserve">degree celsius</t>
   </si>
   <si>
+    <t xml:space="preserve">Thermometrics Climate RTD 100 ohm Probe, housed within a Met One 076B fan aspirated radiation shield </t>
+  </si>
+  <si>
     <t xml:space="preserve">DP1.00003.001</t>
   </si>
   <si>
@@ -157,6 +166,9 @@
     <t xml:space="preserve">DP1.00003.001_tempTripleMean</t>
   </si>
   <si>
+    <t xml:space="preserve">Observations are made by three platinum resistance thermometers, which are housed together in a fan aspirated shield to reduce radiative biases. </t>
+  </si>
+  <si>
     <t xml:space="preserve">DP1.00004.001</t>
   </si>
   <si>
@@ -181,6 +193,9 @@
     <t xml:space="preserve">kilopascal</t>
   </si>
   <si>
+    <t xml:space="preserve">Observations are made by a single digital barometer located on the tower infrastructure and a single digital barometer located on the aquatic meteorological station. </t>
+  </si>
+  <si>
     <t xml:space="preserve">corPres</t>
   </si>
   <si>
@@ -199,7 +214,7 @@
     <t xml:space="preserve">bioTempMean</t>
   </si>
   <si>
-    <t xml:space="preserve">http://data.neonscience.org/api/v0/documents/NEON.DOC.000652vA</t>
+    <t xml:space="preserve">http://data.neonscience.org/api/data-product-view?dpCode=DP1.0005.001</t>
   </si>
   <si>
     <t xml:space="preserve">DP1.00005.001_bioTempMean</t>
@@ -208,6 +223,9 @@
     <t xml:space="preserve">Other</t>
   </si>
   <si>
+    <t xml:space="preserve">Biological temperature (i.e. surface temperature) is measured via Apogee SI-111 infrared (IR) temperature sensor. </t>
+  </si>
+  <si>
     <t xml:space="preserve">DP1.00006.001</t>
   </si>
   <si>
@@ -232,6 +250,9 @@
     <t xml:space="preserve">millimeter</t>
   </si>
   <si>
+    <t xml:space="preserve">Belfort AEPG II 600M weighing gauge (primary precipitation)</t>
+  </si>
+  <si>
     <t xml:space="preserve">SECPRE_30min</t>
   </si>
   <si>
@@ -244,6 +265,9 @@
     <t xml:space="preserve">DP1.00006.001_secPrecipBulk</t>
   </si>
   <si>
+    <t xml:space="preserve">Met One 372 tipping bucket (non-heated) and 379 tipping bucket (heated)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Paused</t>
   </si>
   <si>
@@ -283,6 +307,9 @@
     <t xml:space="preserve">watts per square meter </t>
   </si>
   <si>
+    <t xml:space="preserve">Total, direct, and diffuse shortwave radiation measured via Delta-T Devices SPN1 Sunshine Pyranometer</t>
+  </si>
+  <si>
     <t xml:space="preserve">DP1.00041.001</t>
   </si>
   <si>
@@ -304,6 +331,9 @@
     <t xml:space="preserve">Soil</t>
   </si>
   <si>
+    <t xml:space="preserve">Temperature of the soil at various depth below the soil surface from 2 cm up to 200 cm measured by Thermometrics - Climate RTD 100-ohm Probe</t>
+  </si>
+  <si>
     <t xml:space="preserve">DP1.00094.001</t>
   </si>
   <si>
@@ -331,6 +361,9 @@
     <t xml:space="preserve">dimensionless</t>
   </si>
   <si>
+    <t xml:space="preserve">Soil volumetric water content at various depth below the soil surface from 2 cm up to 200 cm measured by Sentek - EnviroSCAN TriSCAN sensor </t>
+  </si>
+  <si>
     <t xml:space="preserve">DP1.20046.001</t>
   </si>
   <si>
@@ -352,6 +385,9 @@
     <t xml:space="preserve">Surface water</t>
   </si>
   <si>
+    <t xml:space="preserve">Vaisala HUMICAP Humidity and Temperature Probe - HMP 155 </t>
+  </si>
+  <si>
     <t xml:space="preserve">DP1.20004.001</t>
   </si>
   <si>
@@ -361,6 +397,9 @@
     <t xml:space="preserve">DP1.20004.001_staPresMean</t>
   </si>
   <si>
+    <t xml:space="preserve">Vaisala - BAROCAP Digital Barometer PTB330 </t>
+  </si>
+  <si>
     <t xml:space="preserve">DP1.20004.001_corPres</t>
   </si>
   <si>
@@ -391,6 +430,9 @@
     <t xml:space="preserve">meter</t>
   </si>
   <si>
+    <t xml:space="preserve">Sensor based measurement of groundwater elevation calculated from pressure transducer readings in each well </t>
+  </si>
+  <si>
     <t xml:space="preserve">DP1.20016.001</t>
   </si>
   <si>
@@ -409,6 +451,9 @@
     <t xml:space="preserve">DP1.20016.001_surfacewaterElevMean</t>
   </si>
   <si>
+    <t xml:space="preserve">Elevaltion of surface water based on sensor measurements of water pressure </t>
+  </si>
+  <si>
     <t xml:space="preserve">DP1.00024.001</t>
   </si>
   <si>
@@ -430,6 +475,9 @@
     <t xml:space="preserve">Radiation, incoming PAR</t>
   </si>
   <si>
+    <t xml:space="preserve">Kipp and Zonen PQS 1 PAR Quantum Sensor </t>
+  </si>
+  <si>
     <t xml:space="preserve">DP1.00066.001</t>
   </si>
   <si>
@@ -448,6 +496,9 @@
     <t xml:space="preserve">DP1.00066.001_linePARMean</t>
   </si>
   <si>
+    <t xml:space="preserve">Licor LI-191-01 Quantum Line Sensor </t>
+  </si>
+  <si>
     <t xml:space="preserve">DP1.20242.001</t>
   </si>
   <si>
@@ -460,6 +511,9 @@
     <t xml:space="preserve">DP1.20042.001_PARMean</t>
   </si>
   <si>
+    <t xml:space="preserve">Measured at water surface by Kipp and Zonen - PQS1 Sensor</t>
+  </si>
+  <si>
     <t xml:space="preserve">DP1.20261.001</t>
   </si>
   <si>
@@ -473,6 +527,9 @@
   </si>
   <si>
     <t xml:space="preserve">DP1.20261.001_uPARMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measured at water surface on buoy by Kipp and Zonen - PQS1 Sensor</t>
   </si>
   <si>
     <t xml:space="preserve">DP1.00098.001</t>
@@ -583,9 +640,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -613,16 +674,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1048576"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O23" activeCellId="0" sqref="O23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.47"/>
@@ -634,1095 +695,1165 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="77.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="8.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="1" t="n">
+      <c r="L2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="2" t="n">
         <v>119</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
+      <c r="O2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="1" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="K4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>96</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="K5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" s="1" t="n">
+      <c r="L5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="2" t="n">
         <v>96</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="O5" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>170</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>170</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="J8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="N8" s="2" t="n">
+        <v>96</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N5" s="1" t="n">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N6" s="1" t="n">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N7" s="1" t="n">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N8" s="1" t="n">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="K9" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="N9" s="0" t="n">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O9" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="N10" s="0" t="n">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O10" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>80</v>
+        <v>87</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>81</v>
+        <v>17</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>86</v>
+        <v>26</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="N12" s="0" t="n">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O12" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="N13" s="0" t="n">
         <v>96</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O13" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>97</v>
+        <v>106</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>100</v>
+        <v>109</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="N14" s="2" t="n">
+        <v>112</v>
+      </c>
+      <c r="N14" s="3" t="n">
         <v>137</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="N15" s="0" t="n">
         <v>96</v>
       </c>
+      <c r="O15" s="3" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="K16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N16" s="1" t="n">
+      <c r="L16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N16" s="2" t="n">
         <v>170</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N17" s="2" t="n">
+        <v>170</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="J18" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N17" s="1" t="n">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>101</v>
-      </c>
       <c r="K18" s="0" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="N18" s="0" t="n">
         <v>33</v>
       </c>
+      <c r="O18" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="I19" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="K19" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="J19" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>109</v>
-      </c>
       <c r="L19" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="N19" s="0" t="n">
         <v>33</v>
       </c>
+      <c r="O19" s="3" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>134</v>
+        <v>21</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="N20" s="0" t="n">
         <v>33</v>
       </c>
+      <c r="O20" s="3" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>141</v>
+        <v>21</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="N21" s="0" t="n">
         <v>33</v>
       </c>
+      <c r="O21" s="3" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>145</v>
+        <v>21</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="N22" s="0" t="n">
         <v>33</v>
       </c>
+      <c r="O22" s="3" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I23" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="I23" s="0" t="s">
-        <v>135</v>
-      </c>
       <c r="J23" s="0" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="N23" s="0" t="n">
         <v>33</v>
       </c>
+      <c r="O23" s="3" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="N24" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="O24" s="3" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>160</v>
+        <v>179</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="N25" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="O25" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
excluded Barometric pressure from harvested NEON variables.
reason: 80 percent of sites had no available published data.
</commit_message>
<xml_diff>
--- a/NEON/NEONHarvester/settings/neon_variables_lookup.xlsx
+++ b/NEON/NEONHarvester/settings/neon_variables_lookup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="neon_variables" sheetId="1" state="visible" r:id="rId2"/>
@@ -199,6 +199,9 @@
     <t xml:space="preserve">corPres</t>
   </si>
   <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
     <t xml:space="preserve">DP1.00004.001_corPres</t>
   </si>
   <si>
@@ -239,9 +242,6 @@
   </si>
   <si>
     <t xml:space="preserve">http://data.neonscience.org/api/v0/documents/NEON.DOC.000898_DRAFT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
   </si>
   <si>
     <t xml:space="preserve">DP1.00006.001_priPrecipBulk</t>
@@ -583,19 +583,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -676,28 +673,28 @@
   </sheetPr>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O23" activeCellId="0" sqref="O23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="60.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="77.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="8.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.7448979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="60.2040816326531"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="76.4030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1002,10 +999,10 @@
         <v>53</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>50</v>
@@ -1031,28 +1028,28 @@
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>21</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>39</v>
@@ -1061,7 +1058,7 @@
         <v>24</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>26</v>
@@ -1073,42 +1070,42 @@
         <v>96</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>74</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J9" s="0" t="s">
         <v>24</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L9" s="0" t="s">
         <v>26</v>
@@ -1125,10 +1122,10 @@
     </row>
     <row r="10" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>17</v>
@@ -1143,19 +1140,19 @@
         <v>79</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>80</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J10" s="0" t="s">
         <v>24</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>26</v>
@@ -1172,10 +1169,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>82</v>
@@ -1190,11 +1187,12 @@
         <v>85</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>86</v>
       </c>
+      <c r="O11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -1498,7 +1496,7 @@
         <v>131</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>132</v>
@@ -1545,7 +1543,7 @@
         <v>141</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="H19" s="0" t="s">
         <v>142</v>
@@ -1604,7 +1602,7 @@
         <v>24</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L20" s="0" t="s">
         <v>26</v>
@@ -1857,10 +1855,10 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Stránka &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>